<commit_message>
Working on my EDA
</commit_message>
<xml_diff>
--- a/CH-107 Matching Tables.xlsx
+++ b/CH-107 Matching Tables.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58F30B9-5B3F-4707-A9F2-35913F72466E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6124B194-75BB-4C37-8FA6-906200C5D8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
     <sheet name="Alt2" sheetId="3" r:id="rId3"/>
+    <sheet name="EDA" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$H$2:$I$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$H$2:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EDA!$H$2:$I$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$H$2:$I$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="16">
   <si>
     <t>Result</t>
   </si>
@@ -484,8 +486,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -500,8 +502,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="238125" y="2019299"/>
-          <a:ext cx="7277100" cy="3495676"/>
+          <a:off x="215265" y="1878329"/>
+          <a:ext cx="6593205" cy="3707131"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1196,7 +1198,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="9">
+  <wetp:taskpane dockstate="right" visibility="0" width="344" row="9">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1228,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1827,7 +1829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2574513-8361-4543-AA39-746721CDDE95}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -2155,4 +2157,373 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288F3326-6D4F-4F22-8FD9-4448202051C0}">
+  <dimension ref="A1:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="E1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="H1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="10"/>
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8">
+        <v>4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="H6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="8">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D10" s="1"/>
+      <c r="H10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D11" s="1"/>
+      <c r="H11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D12" s="1"/>
+      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" t="str" cm="1">
+        <f t="array" ref="B15:C24">_xlfn.LET(
+    _xlpm.e, B3:C9,
+    _xlpm.m, E3:F9,
+    _xlpm.q, "Q-" &amp; ROW(1:10),
+    _xlfn.HSTACK(_xlpm.q, _xlfn.IFNA(IFERROR((1 / VLOOKUP(_xlpm.q, _xlpm.m, 2, )) ^ -1, VLOOKUP(_xlpm.q, _xlpm.e, 2, )), ""))
+)</f>
+        <v>Q-1</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="E15" cm="1">
+        <f t="array" ref="E15:E24">_xlfn.LET(
+    _xlpm.e, B3:C9,
+    _xlpm.m, E3:F9,
+    _xlpm.q, "Q-" &amp; ROW(1:10),
+    IFERROR((1 / VLOOKUP(_xlpm.q, _xlpm.m, 2, )) ^ -1, VLOOKUP(_xlpm.q, _xlpm.e, 2, )))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <v>Q-2</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="str">
+        <v>Q-3</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <v>Q-4</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <v>Q-5</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <v>Q-6</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <v>Q-7</v>
+      </c>
+      <c r="C21" t="str">
+        <v/>
+      </c>
+      <c r="E21" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <v>Q-8</v>
+      </c>
+      <c r="C22" t="str">
+        <v/>
+      </c>
+      <c r="E22" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <v>Q-9</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <v>Q-10</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="H2:I15" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H3:I15">
+      <sortCondition ref="H2:H15"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>